<commit_message>
EDIT OPTION ADDED AND MAJOR BUGS ARE FIXED
</commit_message>
<xml_diff>
--- a/public/assets/students_template.xlsx
+++ b/public/assets/students_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\React\anits-edu-sphere\frontend\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE1601E-AC50-4710-B20D-8D1AD70CF637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0B02F4-86BC-4060-B06C-03C638B45CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3EB12AA1-D52F-4A7E-8C37-174E52B0913D}"/>
   </bookViews>
@@ -448,12 +448,12 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -522,7 +522,7 @@
         <v>12</v>
       </c>
       <c r="F2">
-        <v>2024009</v>
+        <v>2024010</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>

</xml_diff>